<commit_message>
update manager export to include phone
</commit_message>
<xml_diff>
--- a/Draco/Content/ManagerAddressListTemplate.xlsx
+++ b/Draco/Content/ManagerAddressListTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Player Name</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Team</t>
+  </si>
+  <si>
+    <t>Work Phone</t>
+  </si>
+  <si>
+    <t>Cell Phone</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
   </si>
 </sst>
 </file>
@@ -382,27 +391,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="26.26953125" customWidth="1"/>
-    <col min="3" max="3" width="29.90625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="9.6328125" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" customWidth="1"/>
+    <col min="1" max="5" width="26.26953125" customWidth="1"/>
+    <col min="6" max="6" width="29.90625" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,18 +422,27 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>